<commit_message>
Berechnung und Reports werden richtig erstellt
</commit_message>
<xml_diff>
--- a/UniApplikation/OutputFiles/MissingStudents.xlsx
+++ b/UniApplikation/OutputFiles/MissingStudents.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14565"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5040" windowHeight="10245"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Number</t>
   </si>
@@ -35,202 +35,214 @@
     <t>MissingCourses</t>
   </si>
   <si>
+    <t>Student84</t>
+  </si>
+  <si>
+    <t>Student45</t>
+  </si>
+  <si>
+    <t>Student79</t>
+  </si>
+  <si>
+    <t>Student5</t>
+  </si>
+  <si>
+    <t>Student113</t>
+  </si>
+  <si>
+    <t>Student86</t>
+  </si>
+  <si>
+    <t>Student60</t>
+  </si>
+  <si>
+    <t>Student2</t>
+  </si>
+  <si>
+    <t>Student134</t>
+  </si>
+  <si>
+    <t>Student10</t>
+  </si>
+  <si>
+    <t>Student110</t>
+  </si>
+  <si>
+    <t>Student114</t>
+  </si>
+  <si>
+    <t>Student90</t>
+  </si>
+  <si>
+    <t>Student22</t>
+  </si>
+  <si>
+    <t>Student130</t>
+  </si>
+  <si>
+    <t>Student118</t>
+  </si>
+  <si>
+    <t>Student137</t>
+  </si>
+  <si>
+    <t>Student111</t>
+  </si>
+  <si>
+    <t>Student150</t>
+  </si>
+  <si>
+    <t>Student87</t>
+  </si>
+  <si>
+    <t>Student148</t>
+  </si>
+  <si>
+    <t>Student109</t>
+  </si>
+  <si>
+    <t>Student49</t>
+  </si>
+  <si>
+    <t>Student139</t>
+  </si>
+  <si>
+    <t>Student36</t>
+  </si>
+  <si>
+    <t>Student50</t>
+  </si>
+  <si>
+    <t>Student141</t>
+  </si>
+  <si>
+    <t>Student125</t>
+  </si>
+  <si>
+    <t>Student37</t>
+  </si>
+  <si>
+    <t>Student77</t>
+  </si>
+  <si>
+    <t>Student33</t>
+  </si>
+  <si>
+    <t>Student115</t>
+  </si>
+  <si>
+    <t>Student132</t>
+  </si>
+  <si>
+    <t>Student51</t>
+  </si>
+  <si>
+    <t>Student92</t>
+  </si>
+  <si>
+    <t>Student129</t>
+  </si>
+  <si>
+    <t>Student53</t>
+  </si>
+  <si>
+    <t>Student35</t>
+  </si>
+  <si>
+    <t>Student131</t>
+  </si>
+  <si>
+    <t>Student18</t>
+  </si>
+  <si>
+    <t>Student81</t>
+  </si>
+  <si>
+    <t>Student102</t>
+  </si>
+  <si>
+    <t>Student94</t>
+  </si>
+  <si>
+    <t>Student103</t>
+  </si>
+  <si>
+    <t>Student143</t>
+  </si>
+  <si>
+    <t>Student70</t>
+  </si>
+  <si>
+    <t>Student121</t>
+  </si>
+  <si>
+    <t>Student127</t>
+  </si>
+  <si>
+    <t>Student48</t>
+  </si>
+  <si>
+    <t>Student107</t>
+  </si>
+  <si>
+    <t>Student74</t>
+  </si>
+  <si>
+    <t>Student126</t>
+  </si>
+  <si>
+    <t>Student93</t>
+  </si>
+  <si>
+    <t>Student42</t>
+  </si>
+  <si>
+    <t>Student61</t>
+  </si>
+  <si>
+    <t>Student38</t>
+  </si>
+  <si>
+    <t>Student23</t>
+  </si>
+  <si>
+    <t>Student106</t>
+  </si>
+  <si>
+    <t>Student78</t>
+  </si>
+  <si>
+    <t>Student122</t>
+  </si>
+  <si>
+    <t>Student76</t>
+  </si>
+  <si>
+    <t>Student34</t>
+  </si>
+  <si>
     <t>Student116</t>
   </si>
   <si>
-    <t>Student70</t>
-  </si>
-  <si>
-    <t>Student132</t>
-  </si>
-  <si>
-    <t>Student60</t>
-  </si>
-  <si>
-    <t>Student126</t>
+    <t>Student138</t>
+  </si>
+  <si>
+    <t>Student98</t>
+  </si>
+  <si>
+    <t>Student62</t>
+  </si>
+  <si>
+    <t>Student80</t>
   </si>
   <si>
     <t>Student100</t>
   </si>
   <si>
-    <t>Student105</t>
-  </si>
-  <si>
-    <t>Student127</t>
-  </si>
-  <si>
-    <t>Student130</t>
-  </si>
-  <si>
-    <t>Student99</t>
-  </si>
-  <si>
-    <t>Student34</t>
-  </si>
-  <si>
-    <t>Student145</t>
-  </si>
-  <si>
-    <t>Student41</t>
-  </si>
-  <si>
-    <t>Student35</t>
-  </si>
-  <si>
-    <t>Student74</t>
-  </si>
-  <si>
-    <t>Student109</t>
-  </si>
-  <si>
-    <t>Student139</t>
-  </si>
-  <si>
-    <t>Student131</t>
-  </si>
-  <si>
-    <t>Student122</t>
-  </si>
-  <si>
-    <t>Student2</t>
-  </si>
-  <si>
-    <t>Student23</t>
-  </si>
-  <si>
-    <t>Student115</t>
-  </si>
-  <si>
-    <t>Student107</t>
-  </si>
-  <si>
-    <t>Student48</t>
-  </si>
-  <si>
-    <t>Student94</t>
-  </si>
-  <si>
-    <t>Student75</t>
-  </si>
-  <si>
-    <t>Student143</t>
-  </si>
-  <si>
-    <t>Student113</t>
-  </si>
-  <si>
-    <t>Student5</t>
-  </si>
-  <si>
-    <t>Student146</t>
-  </si>
-  <si>
-    <t>Student102</t>
-  </si>
-  <si>
-    <t>Student147</t>
-  </si>
-  <si>
-    <t>Student61</t>
-  </si>
-  <si>
-    <t>Student51</t>
-  </si>
-  <si>
-    <t>Student140</t>
-  </si>
-  <si>
-    <t>Student36</t>
-  </si>
-  <si>
-    <t>Student62</t>
-  </si>
-  <si>
-    <t>Student50</t>
-  </si>
-  <si>
-    <t>Student111</t>
-  </si>
-  <si>
-    <t>Student53</t>
-  </si>
-  <si>
-    <t>Student79</t>
-  </si>
-  <si>
-    <t>Student78</t>
-  </si>
-  <si>
-    <t>Student22</t>
-  </si>
-  <si>
-    <t>Student134</t>
-  </si>
-  <si>
-    <t>Student81</t>
+    <t>Student142</t>
   </si>
   <si>
     <t>Student54</t>
-  </si>
-  <si>
-    <t>Student103</t>
-  </si>
-  <si>
-    <t>Student129</t>
-  </si>
-  <si>
-    <t>Student10</t>
-  </si>
-  <si>
-    <t>Student108</t>
-  </si>
-  <si>
-    <t>Student106</t>
-  </si>
-  <si>
-    <t>Student150</t>
-  </si>
-  <si>
-    <t>Student18</t>
-  </si>
-  <si>
-    <t>Student84</t>
-  </si>
-  <si>
-    <t>Student86</t>
-  </si>
-  <si>
-    <t>Student77</t>
-  </si>
-  <si>
-    <t>Student114</t>
-  </si>
-  <si>
-    <t>Student141</t>
-  </si>
-  <si>
-    <t>Student80</t>
-  </si>
-  <si>
-    <t>Student142</t>
-  </si>
-  <si>
-    <t>Student138</t>
-  </si>
-  <si>
-    <t>Student38</t>
-  </si>
-  <si>
-    <t>Student110</t>
-  </si>
-  <si>
-    <t>Student76</t>
-  </si>
-  <si>
-    <t>Student98</t>
-  </si>
-  <si>
-    <t>Student93</t>
   </si>
 </sst>
 </file>
@@ -548,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -573,7 +585,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -584,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,7 +673,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,7 +684,7 @@
         <v>12</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,7 +717,7 @@
         <v>15</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,7 +739,7 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -738,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -804,7 +816,7 @@
         <v>24</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +882,7 @@
         <v>30</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,7 +904,7 @@
         <v>32</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,7 +915,7 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +926,7 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,7 +981,7 @@
         <v>39</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1036,7 @@
         <v>44</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1068,7 +1080,7 @@
         <v>48</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,7 +1113,7 @@
         <v>51</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,7 +1135,7 @@
         <v>53</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,7 +1168,7 @@
         <v>56</v>
       </c>
       <c r="C55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,7 +1179,7 @@
         <v>57</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1190,7 @@
         <v>58</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1244,7 +1256,7 @@
         <v>64</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1288,6 +1300,50 @@
         <v>68</v>
       </c>
       <c r="C67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
         <v>1</v>
       </c>
     </row>

</xml_diff>